<commit_message>
Finished the dairy products, almost done dairy aisle, needs banner.
</commit_message>
<xml_diff>
--- a/grocerySpreadsheet.xlsx
+++ b/grocerySpreadsheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\Grocery\grocery_website\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\Web Project SOEN 287\grocery_website\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4310745F-DD10-412B-8566-645DC7B59099}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{082F305F-12DE-46DA-9571-5C4FDE23DA92}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2460" yWindow="528" windowWidth="17280" windowHeight="11184" xr2:uid="{64097459-6729-4507-9900-8D24C8A0A9BC}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{64097459-6729-4507-9900-8D24C8A0A9BC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,6 @@
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -34,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Name</t>
   </si>
@@ -67,6 +66,9 @@
   </si>
   <si>
     <t>Carson Senthilkumar</t>
+  </si>
+  <si>
+    <t>Created the shopping cart page (p4), Created the Dairy Aisle and the dairy products (p2 and p3), and created the back page edit product page (p8). Also worked on CSS relating to the pages created (created a few classes to make the receipt display properly for example).</t>
   </si>
 </sst>
 </file>
@@ -467,7 +469,7 @@
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -515,7 +517,9 @@
       <c r="B4" s="5">
         <v>40168674</v>
       </c>
-      <c r="C4" s="1"/>
+      <c r="C4" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>

</xml_diff>

<commit_message>
added p3 pages for produce, added banners for dairy and candy, and adjusted banners for mobile view
</commit_message>
<xml_diff>
--- a/grocerySpreadsheet.xlsx
+++ b/grocerySpreadsheet.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\Web Project SOEN 287\grocery_website\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yangt\Documents\School\Concordia\Winter 2021\SOEN 287\grocery_website\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{082F305F-12DE-46DA-9571-5C4FDE23DA92}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C01716C-D7DF-4981-9AD2-6D4FEC494152}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{64097459-6729-4507-9900-8D24C8A0A9BC}"/>
+    <workbookView xWindow="3810" yWindow="3630" windowWidth="21600" windowHeight="11385" xr2:uid="{64097459-6729-4507-9900-8D24C8A0A9BC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Name</t>
   </si>
@@ -69,6 +69,9 @@
   </si>
   <si>
     <t>Created the shopping cart page (p4), Created the Dairy Aisle and the dairy products (p2 and p3), and created the back page edit product page (p8). Also worked on CSS relating to the pages created (created a few classes to make the receipt display properly for example).</t>
+  </si>
+  <si>
+    <t>Created template for P2 pages. Made banners for P2 pages. Created Produce aisle (P2), product descriptions for Produce aisle (P3), P5 and P6. Worked on CSS for the pages created.</t>
   </si>
 </sst>
 </file>
@@ -469,17 +472,17 @@
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.21875" customWidth="1"/>
+    <col min="1" max="1" width="16.28515625" customWidth="1"/>
     <col min="2" max="2" width="10" customWidth="1"/>
-    <col min="3" max="3" width="73.5546875" customWidth="1"/>
+    <col min="3" max="3" width="73.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -490,7 +493,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="106.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="106.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -504,13 +507,13 @@
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -524,22 +527,25 @@
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
     </row>
-    <row r="5" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
     </row>
-    <row r="6" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B6" s="4">
         <v>40171440</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="8" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C6" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="8" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>7</v>
       </c>
@@ -547,8 +553,8 @@
         <v>40174018</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="10" spans="1:6" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="10" spans="1:6" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>8</v>
       </c>

</xml_diff>

<commit_message>
Fixed links and finished candy edit.
</commit_message>
<xml_diff>
--- a/grocerySpreadsheet.xlsx
+++ b/grocerySpreadsheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\Grocery\grocery_website\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\Web Project SOEN 287\grocery_website\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D9CE54C-8D38-47D8-8504-7CE1F2F891C3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F96AE55-6218-4F10-85EC-BA9309BAD44A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{64097459-6729-4507-9900-8D24C8A0A9BC}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{64097459-6729-4507-9900-8D24C8A0A9BC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -59,13 +59,16 @@
     <t>Carson Senthilkumar</t>
   </si>
   <si>
-    <t>Created the shopping cart page (p4), Created the Dairy Aisle and the dairy products (p2 and p3), and created the back page edit product page (p8). Also worked on CSS relating to the pages created (created a few classes to make the receipt display properly for example).</t>
-  </si>
-  <si>
-    <t>Created template for P2 pages. Made banners for P2 pages. Created Produce aisle (P2), product descriptions for Produce aisle (P3), P5 and P6. Worked on CSS for the pages created.</t>
-  </si>
-  <si>
     <t>Homepage P1 (index.html) and everything therein, including the banners, food displays, buttons, and basic styles that are applied elsewhere. Also made P2 grain aisle page and all P3 pages relating to grain foods. I made the user edit page. I also handled hosting of the website and I was the Github administrator, responsible for handling merge conflicts and other issues.</t>
+  </si>
+  <si>
+    <t>Created the shopping cart page (p4), Created the Dairy Aisle and the dairy products (p2 and p3), and created the back page edit product pages (p8).
+ Also worked on CSS relating to the pages created (created a few classes to make the
+ receipt display properly for example).</t>
+  </si>
+  <si>
+    <t>Created template for P2 pages. Made banners for P2 pages.
+ Created Produce aisle (P2), product descriptions for Produce aisle (P3), P5 and P6. Worked on CSS for the pages created.</t>
   </si>
 </sst>
 </file>
@@ -134,7 +137,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -149,6 +152,9 @@
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -466,7 +472,7 @@
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -495,7 +501,7 @@
         <v>40170301</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
@@ -507,15 +513,15 @@
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" ht="61.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="5">
         <v>40168674</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>8</v>
+      <c r="C4" s="6" t="s">
+        <v>9</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
@@ -527,15 +533,15 @@
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
     </row>
-    <row r="6" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" ht="56.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="4">
         <v>40171440</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>9</v>
+      <c r="C6" s="6" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
FINAL COMMIT for part 1. Fix thankyou.html broken link.
</commit_message>
<xml_diff>
--- a/grocerySpreadsheet.xlsx
+++ b/grocerySpreadsheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\Grocery\grocery_website\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38C275DF-DEFB-433E-A63B-705FE3DFC8E3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{367C669E-B654-4C79-A689-5E61C21848A4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{64097459-6729-4507-9900-8D24C8A0A9BC}"/>
   </bookViews>
@@ -59,9 +59,6 @@
     <t>Carson Senthilkumar</t>
   </si>
   <si>
-    <t>Homepage P1 (index.html) and everything therein, including the banners, food displays, buttons, and basic styles that are applied elsewhere. Also made P2 grain aisle page and all P3 pages relating to grain foods. I made the user edit page. I also handled hosting of the website and I was the Github administrator, responsible for handling merge conflicts and other issues.</t>
-  </si>
-  <si>
     <t>Created the shopping cart page (p4), Created the Dairy Aisle and the dairy products (p2 and p3), and created the back page edit product pages (p8).
  Also worked on CSS relating to the pages created (created a few classes to make the
  receipt display properly for example).</t>
@@ -71,14 +68,17 @@
  Created Produce aisle (P2), product descriptions for Produce aisle (P3), P5 and P6. Worked on CSS for the pages created.</t>
   </si>
   <si>
-    <t>Created a template for back end function lists and edit. Created the userlist page (P7) 
-and edit an order profile page (P12). Created the meat aisle (P2) and meat production 
-description page (P3). Created the CSS related to those pages.</t>
-  </si>
-  <si>
     <t>Created the Candy aisle (P2) , the candy product description for each item of the candy 
 aisle (P3) , the product list for all products listed on the website(P7)
  and the order list page (p11).</t>
+  </si>
+  <si>
+    <t>Created a template for back end function lists and edit. Created the userlist page (P9) 
+and edit an order profile page (P12). Created the meat aisle (P2) and meat product 
+description page (P3). Created the CSS related to those pages.</t>
+  </si>
+  <si>
+    <t>Homepage (P1) (index.html) and everything therein, including the banners, food displays, buttons, and basic styles that are applied elsewhere. Also made (P2) grain aisle page and all (P3) pages relating to grain foods. I made the user edit page (P10). I also handled hosting of the website and I was the Github administrator, responsible for handling merge conflicts and other issues.</t>
   </si>
 </sst>
 </file>
@@ -490,7 +490,7 @@
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -519,7 +519,7 @@
         <v>40170301</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
@@ -539,7 +539,7 @@
         <v>40168674</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
@@ -559,7 +559,7 @@
         <v>40171440</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
@@ -583,7 +583,7 @@
         <v>40173515</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>